<commit_message>
update file system typos
</commit_message>
<xml_diff>
--- a/file-system/all_obs/summary_obs.xlsx
+++ b/file-system/all_obs/summary_obs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Project\observations\projecta_2022-03-13\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crystal\Desktop\desktop\R\Working R Stuff\data-wrangling-functions\file-system\obs_2023-01-18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C05FF6A7-F3C4-44C7-86F5-C06FDB8FEA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B013C31-F87E-4679-B6E6-6E7B00F8CB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1D94EB9F-5C4D-4FD2-97BF-9281BE394235}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{1D94EB9F-5C4D-4FD2-97BF-9281BE394235}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,15 +395,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B233E95-6B38-4F01-982C-B4EDAD5E6D4B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D11:D12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -425,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -436,7 +436,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -445,6 +445,11 @@
       </c>
       <c r="C4">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>